<commit_message>
Agrego cosas que no se han commiteado previamente y no entraron en los pushes
</commit_message>
<xml_diff>
--- a/Primera Entrega/Clase 9- Cierre Estructura/Alumnos/Gabriel Nogueira/Actividad 9.xlsx
+++ b/Primera Entrega/Clase 9- Cierre Estructura/Alumnos/Gabriel Nogueira/Actividad 9.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\Mochila_C80522\Primera Entrega\Clase 9- Cierre Estructura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\Mochila_C80522\Primera Entrega\Clase 9- Cierre Estructura\Alumnos\Gabriel Nogueira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3890B7BA-1143-49A7-AFF0-6EA99152FFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EBBED5-AE4B-4F01-9F4E-23F59F087789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,66 +25,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
-  <si>
-    <t>Gama Baja</t>
-  </si>
-  <si>
-    <t>Intel</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>A criterio</t>
-  </si>
-  <si>
-    <t>Core i3 7100</t>
-  </si>
-  <si>
-    <t>Placa Madre</t>
-  </si>
-  <si>
-    <t>Memoria Principal</t>
-  </si>
-  <si>
-    <t>Memoria Secundaria</t>
-  </si>
-  <si>
-    <t>Procesador</t>
-  </si>
-  <si>
-    <t>Ryzen 3 2200g</t>
-  </si>
-  <si>
-    <t>HDD 1TB SATA3 WD BLUE</t>
-  </si>
-  <si>
-    <t>DDR4 4GB 2400 MARKVISION 1.20V</t>
-  </si>
-  <si>
-    <t>GIGABYTE H610M S2H DDR4 S1700</t>
-  </si>
-  <si>
-    <t>CELERON G6900 S1700</t>
-  </si>
-  <si>
-    <t>Gama Media</t>
-  </si>
-  <si>
-    <t>MICRO AMD RYZEN 5 5600X</t>
-  </si>
-  <si>
-    <t>MOTHER B550 PRO</t>
-  </si>
-  <si>
-    <t>MEMORIA 8GB DDR4 2666MHZ x 2</t>
-  </si>
-  <si>
-    <t>DISCO HDD 1TB SATA III</t>
-  </si>
-  <si>
-    <t>VIDEO GEFORCE GTX 1660 SUPER 6GB</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+  <si>
+    <t>gama baja intel</t>
+  </si>
+  <si>
+    <t>Procesador          Core i3 7100</t>
+  </si>
+  <si>
+    <t>Placa madre         asrock h110m-hdv r3.0</t>
+  </si>
+  <si>
+    <t>Memoria principal   KINGSTON 4GB DDR4 2400 MHz</t>
+  </si>
+  <si>
+    <t>Memoria secundaria  Disco Rigido 500gb Blue Wd Western Digital 64mb Mallweb 500gb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gama baja amd </t>
+  </si>
+  <si>
+    <t>Procesador          Ryzen 3 2200g</t>
+  </si>
+  <si>
+    <t>Placa madre         GIGABYTE B450M DS3H</t>
+  </si>
+  <si>
+    <t>Memoria ram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Memoria RAM Fury Beast DDR4 8GB 1 Kingston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gama baja </t>
+  </si>
+  <si>
+    <t>Procesador          INTEL CELERON G6900 S1700</t>
+  </si>
+  <si>
+    <t>Placa madre         GIGABYTE H610M S2H DDR4 S1700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  DDR4 4GB 2400 MARKVISION 1.20V</t>
+  </si>
+  <si>
+    <t>Memoria secundaria  HDD 1TB SATA3 WD BLUE</t>
+  </si>
+  <si>
+    <t>-----------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>gama media intel</t>
+  </si>
+  <si>
+    <t>Procesador          INTEL CORE I5 11400F S/VIDEO</t>
+  </si>
+  <si>
+    <t>Placa madre         ASUS PRIME B560M-A(x 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  8GB DDR4 3200MHZ PATRIOT SIGNATURE LINE</t>
+  </si>
+  <si>
+    <t>Memoria secundaria  HD SSD 240GB WD GREEN SATA III 2.5"</t>
+  </si>
+  <si>
+    <t>gpu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  GeForce GT 1030 2GD4 LP OC</t>
+  </si>
+  <si>
+    <t>Procesador          AMD A10 9700</t>
+  </si>
+  <si>
+    <t>Placa madre         A320M Asrock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  DDR4 16GB 3000 MHz (1x16GB)</t>
+  </si>
+  <si>
+    <t>Memoria secundaria  SSD de 240 gb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEFORCE GTX 1660 SUPER 6GB</t>
+  </si>
+  <si>
+    <t>Procesador          AMD RYZEN 5 5600X</t>
+  </si>
+  <si>
+    <t>Placa madre         B550 PRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  8GB DDR4 2666MHZ x 2</t>
+  </si>
+  <si>
+    <t>Memoria secundaria  HDD 1TB SATA III</t>
+  </si>
+  <si>
+    <t>---------------------------------------------------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gama alta intel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procesador         CORE I7 10700K </t>
+  </si>
+  <si>
+    <t>Placa madre        ASROCK Z590 OC FORMULA DDR4 S1200</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16GB (2X8GB) DDR4 3733 GIGABYTE AORUS RGB DEMO KIT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memoria secundaria 1TB PNY CS3040 M2 NVME GEN4 CON DISIPADOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       GEFORCE RTX 3080 10GB AFOX MINING NO-LHR</t>
+  </si>
+  <si>
+    <t>gama alta amd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procesador         Amd Ryzen 7 3800xt </t>
+  </si>
+  <si>
+    <t>Placa madre         Madre ASRock A320M-HDV R4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16GB (2X8GB) DDR4 3733 GIGABYTE AORUS RGB DEMO KIT  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memoria secundaria 1TB PNY CS3040 M2 NVME GEN4 CON DISIPADOR  </t>
+  </si>
+  <si>
+    <t>gama alta</t>
+  </si>
+  <si>
+    <t>Procesador          INTEL CORE I9 12900K S/COOLER S1700(x 1)</t>
+  </si>
+  <si>
+    <t>Placa madre         GIGABYTE Z690 AORUS MASTER DDR5(x 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  32GB (2X16GB) DDR5 5200 GIGABYTE AORUS(x 1)</t>
+  </si>
+  <si>
+    <t>Memoria secundaria  HD SSD 2TB GIGABYTE AORUS PCIE CARD 3D GEN4(x 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEFORCE RTX 3080 10GB AFOX MINING NO-LHR</t>
   </si>
 </sst>
 </file>
@@ -125,11 +215,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -414,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -429,108 +516,320 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="D11" s="3" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="D12" t="s">
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="D13" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="D14" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>